<commit_message>
done fix import vat tu
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/MauFileVatTu.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/MauFileVatTu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMT\source\repos\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAI\source\repos\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA728BA-2FD1-4AAC-84FA-7CD6B2AE3B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>GIGA</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Tên vật tư</t>
   </si>
@@ -70,12 +71,24 @@
   </si>
   <si>
     <t>Giá mua</t>
+  </si>
+  <si>
+    <t>Đơn vị mặc định</t>
+  </si>
+  <si>
+    <t>Đơn vị mua</t>
+  </si>
+  <si>
+    <t>Mức tồn tối thiểu</t>
+  </si>
+  <si>
+    <t>Cái</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,11 +417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,9 +430,12 @@
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +448,17 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -445,6 +470,15 @@
       </c>
       <c r="D2" s="3">
         <v>150000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>